<commit_message>
add NG_CONNTENT IN IQA TABLE
</commit_message>
<xml_diff>
--- a/Reference/INTPUT_TEST_2018_1.xlsx
+++ b/Reference/INTPUT_TEST_2018_1.xlsx
@@ -5711,6 +5711,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5727,21 +5742,6 @@
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1938">
@@ -8109,29 +8109,29 @@
     <row r="1" spans="1:14" s="17" customFormat="1" ht="51" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="43" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="43"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:14" s="17" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="15"/>
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="20"/>
       <c r="K2" s="21"/>
       <c r="M2" s="22" t="s">
@@ -8142,16 +8142,16 @@
       <c r="A3" s="23"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="46" t="s">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8165,10 +8165,10 @@
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="47" t="s">
+      <c r="K4" s="42" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="8" t="s">
@@ -8179,19 +8179,19 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="54" customHeight="1" thickBot="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="H5" s="10"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="43" t="s">
         <v>23</v>
       </c>
       <c r="M5" s="12" t="s">
@@ -8229,10 +8229,10 @@
       <c r="I6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="40" t="s">
         <v>2</v>
       </c>
       <c r="M6" s="9" t="s">

</xml_diff>